<commit_message>
Aula de modulos - openpyxl
</commit_message>
<xml_diff>
--- a/4-Modulos_Python/23-openpyxl/pedidos.xlsx
+++ b/4-Modulos_Python/23-openpyxl/pedidos.xlsx
@@ -125,7 +125,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -138,7 +138,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,10 +174,10 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="19.31"/>
@@ -194,7 +202,7 @@
       <c r="B2" s="3" t="n">
         <v>1002</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="4" t="n">
         <v>50</v>
       </c>
       <c r="D2" s="2"/>
@@ -206,7 +214,7 @@
       <c r="B3" s="3" t="n">
         <v>1005</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <v>32.25</v>
       </c>
       <c r="D3" s="2"/>
@@ -218,7 +226,7 @@
       <c r="B4" s="3" t="n">
         <v>1200</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <v>89.99</v>
       </c>
       <c r="D4" s="2"/>
@@ -226,92 +234,92 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>